<commit_message>
PDF collected during start of Studio 1
</commit_message>
<xml_diff>
--- a/NIS_Compliance_Chart.xlsx
+++ b/NIS_Compliance_Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\home\operations\Studies\Studio1_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu20Prod\home\operations\Studies\Studio1_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9C8CD3-BCD2-4E44-B363-17924E78BCA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE18A044-35A3-45A9-80D5-48C4B5F122D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="17205" windowWidth="24600" windowHeight="15195" xr2:uid="{19B11952-06F8-4DA0-ADF5-9EBA53337F64}"/>
+    <workbookView xWindow="7410" yWindow="8010" windowWidth="28800" windowHeight="23535" xr2:uid="{19B11952-06F8-4DA0-ADF5-9EBA53337F64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>National provision to implement supervision of critical infrastructure</t>
   </si>
@@ -280,7 +280,10 @@
 Danish While the Danish Armed Forces aims to increase its capacity to engage with military cyber operations.</t>
   </si>
   <si>
-    <t>Netherlands</t>
+    <t>Undetermined</t>
+  </si>
+  <si>
+    <t>NCSS states that entities who provisions Essential Services or manages Critical Infrastructures are the ones responsible to implement appropriate measure for Cyber Security.</t>
   </si>
 </sst>
 </file>
@@ -730,6 +733,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -739,18 +811,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -759,103 +819,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1083,10 +1052,44 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <right style="thin">
           <color indexed="64"/>
         </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1103,23 +1106,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0AEB7E4D-4BD4-4436-A9F1-A5C67A12ACFC}" name="Table2" displayName="Table2" ref="B4:O14" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0AEB7E4D-4BD4-4436-A9F1-A5C67A12ACFC}" name="Table2" displayName="Table2" ref="B4:O14" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="B4:O14" xr:uid="{F285111F-7F93-4D4F-8F65-5A0D17A5D31B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{9B7EE70C-7DB7-4740-8F7D-D45BF5411602}" name="Column1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{D15AC0C6-D15D-4A53-94FE-8BB5C384AEE0}" name="Column2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2EB7D748-869F-4BE6-8517-549700BB067E}" name="Column3" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{45E2C6DA-E66D-4B8B-98B5-49A9A8A6CF6D}" name="Column4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{0B229145-8970-4DB7-9E28-8A5F42EEE2F7}" name="Column5" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{15B29F42-9913-43A8-981C-A94F7984E307}" name="Column6" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{B4DF96BC-CBFC-4A59-ABAF-5860AD6F2186}" name="Column7" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{797E1E13-03C9-4D0D-A193-4482BFF07D4E}" name="Column8" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{A776693C-24D0-418F-9B17-01DE356FA816}" name="Column9" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{E499937B-CF62-4BA2-81D9-4A1ABF266284}" name="Column10" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{C19E6C32-50F1-4D26-ABA9-81ED028D97C5}" name="Column11" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{1EEFBDC2-1462-4D0D-9B25-50FC861DF205}" name="Column12" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{C85A34A5-398A-490D-A40E-54FBF3EBF425}" name="Column13" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{1A43C473-BA23-4998-8C0C-6ED4A9E40310}" name="Column14" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{9B7EE70C-7DB7-4740-8F7D-D45BF5411602}" name="Column1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{D15AC0C6-D15D-4A53-94FE-8BB5C384AEE0}" name="Column2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{2EB7D748-869F-4BE6-8517-549700BB067E}" name="Column3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{45E2C6DA-E66D-4B8B-98B5-49A9A8A6CF6D}" name="Column4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{0B229145-8970-4DB7-9E28-8A5F42EEE2F7}" name="Column5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{15B29F42-9913-43A8-981C-A94F7984E307}" name="Column6" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{B4DF96BC-CBFC-4A59-ABAF-5860AD6F2186}" name="Column7" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{797E1E13-03C9-4D0D-A193-4482BFF07D4E}" name="Column8" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{A776693C-24D0-418F-9B17-01DE356FA816}" name="Column9" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{E499937B-CF62-4BA2-81D9-4A1ABF266284}" name="Column10" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{C19E6C32-50F1-4D26-ABA9-81ED028D97C5}" name="Column11" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{1EEFBDC2-1462-4D0D-9B25-50FC861DF205}" name="Column12" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{C85A34A5-398A-490D-A40E-54FBF3EBF425}" name="Column13" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{1A43C473-BA23-4998-8C0C-6ED4A9E40310}" name="Column14" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1422,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9FF0FC-BE56-4B85-B603-AB588A5F9FED}">
-  <dimension ref="B2:V28"/>
+  <dimension ref="B2:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,65 +1438,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="20"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="2:22" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="M3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="1"/>
@@ -1504,72 +1507,72 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="2:22" s="2" customFormat="1" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="36" t="s">
+      <c r="O4" s="27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:22" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+    <row r="5" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="36"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="27"/>
     </row>
-    <row r="6" spans="2:22" s="2" customFormat="1" ht="345" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="2:22" s="2" customFormat="1" ht="345" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1608,12 +1611,12 @@
       <c r="N6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="37" t="s">
+      <c r="O6" s="28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:22" s="2" customFormat="1" ht="345" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+    <row r="7" spans="2:22" s="2" customFormat="1" ht="345" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1640,10 +1643,10 @@
       <c r="L7" s="3"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="37"/>
+      <c r="O7" s="28"/>
     </row>
-    <row r="8" spans="2:22" s="2" customFormat="1" ht="135.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+    <row r="8" spans="2:22" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1662,10 +1665,10 @@
       <c r="L8" s="3"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="37"/>
+      <c r="O8" s="28"/>
     </row>
     <row r="9" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1682,10 +1685,10 @@
       <c r="L9" s="3"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="37"/>
+      <c r="O9" s="28"/>
     </row>
     <row r="10" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1702,10 +1705,10 @@
       <c r="L10" s="3"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="37"/>
+      <c r="O10" s="28"/>
     </row>
     <row r="11" spans="2:22" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1724,10 +1727,10 @@
       <c r="L11" s="3"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="37"/>
+      <c r="O11" s="28"/>
     </row>
     <row r="12" spans="2:22" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="30" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1748,13 +1751,15 @@
       <c r="L12" s="3"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="37"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13" spans="2:22" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1766,75 +1771,41 @@
       <c r="L13" s="3"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="37"/>
+      <c r="O13" s="28"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+    <row r="14" spans="2:22" ht="105" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
+      <c r="C14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="K14" s="10"/>
       <c r="L14" s="6"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="38"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
+      <c r="O14" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>